<commit_message>
#add component show detail rate
</commit_message>
<xml_diff>
--- a/ME-API/Resources/Template/SME_Score_Record_Template.xlsx
+++ b/ME-API/Resources/Template/SME_Score_Record_Template.xlsx
@@ -106,8 +106,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -179,11 +180,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +470,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,21 +491,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -547,8 +548,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">

</xml_diff>